<commit_message>
Added list of variable names when loading DataFrame
</commit_message>
<xml_diff>
--- a/Tests/Dummy Data.xlsx
+++ b/Tests/Dummy Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisonprice/Documents/University/Transform Law KWM Prize/Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DE700D-45D6-B246-9CE7-149BC8A5D059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8771C580-F498-6646-979E-25747ED75AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{103ACD5B-017B-416E-9490-7DFD75D386FE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Client</t>
   </si>
@@ -61,7 +61,19 @@
     <t>CHECK</t>
   </si>
   <si>
-    <t>Existing Client? (1) yes, (0) no</t>
+    <t>Testementary Trust</t>
+  </si>
+  <si>
+    <t>Multiple national jurisdictions</t>
+  </si>
+  <si>
+    <t>Beneficiaries</t>
+  </si>
+  <si>
+    <t>Existing client</t>
+  </si>
+  <si>
+    <t>Claims expected against estate</t>
   </si>
 </sst>
 </file>
@@ -485,7 +497,7 @@
       </c>
       <c r="E3">
         <f ca="1">RANDBETWEEN(1,15)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(0,1)</f>
@@ -493,7 +505,7 @@
       </c>
       <c r="G3">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f ca="1">RANDBETWEEN(0,1)</f>
@@ -501,7 +513,7 @@
       </c>
       <c r="I3">
         <f ca="1">((RANDBETWEEN(10,15)/10)*D3)+(RANDBETWEEN(10,100)*E3)+(20000*F3)+(10000*G3)+(10000*H3)-(5000*C3)</f>
-        <v>725783</v>
+        <v>785132</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -516,7 +528,7 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E67" ca="1" si="0">RANDBETWEEN(1,15)</f>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:H67" ca="1" si="1">RANDBETWEEN(0,1)</f>
@@ -524,15 +536,15 @@
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I35" ca="1" si="2">((RANDBETWEEN(10,15)/10)*D4)+(RANDBETWEEN(2000,4000)*E4)+(50000*F4)+(10000*G4)+(10000*H4)-(5000*C4)</f>
-        <v>301564</v>
+        <v>288102</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
@@ -547,11 +559,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="1"/>
@@ -559,11 +571,11 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="2"/>
-        <v>1276300</v>
+        <v>1027338</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
@@ -578,7 +590,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
@@ -590,11 +602,11 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="2"/>
-        <v>750673</v>
+        <v>918554</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
@@ -609,23 +621,23 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="2"/>
-        <v>684850</v>
+        <v>498110</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
@@ -640,7 +652,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
@@ -656,7 +668,7 @@
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="2"/>
-        <v>13080564</v>
+        <v>12099295</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -668,11 +680,11 @@
       </c>
       <c r="D9">
         <f ca="1">RANDBETWEEN(100,10000)*1000</f>
-        <v>8393000</v>
+        <v>160000</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
@@ -688,7 +700,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="2"/>
-        <v>10953839</v>
+        <v>246546</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -700,11 +712,11 @@
       </c>
       <c r="D10">
         <f t="shared" ref="D10:D73" ca="1" si="3">RANDBETWEEN(100,10000)*1000</f>
-        <v>8045000</v>
+        <v>9601000</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
@@ -712,7 +724,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
@@ -720,7 +732,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="2"/>
-        <v>8902924</v>
+        <v>14482460</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -732,27 +744,27 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="3"/>
-        <v>769000</v>
+        <v>5079000</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="2"/>
-        <v>1032783</v>
+        <v>7183186</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -764,11 +776,11 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="3"/>
-        <v>510000</v>
+        <v>6809000</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
@@ -776,7 +788,7 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
@@ -784,7 +796,7 @@
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="2"/>
-        <v>639475</v>
+        <v>6846035</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -796,11 +808,11 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="3"/>
-        <v>4166000</v>
+        <v>1542000</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
@@ -812,11 +824,11 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="2"/>
-        <v>4620250</v>
+        <v>2160949</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
@@ -828,11 +840,11 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="3"/>
-        <v>7842000</v>
+        <v>208000</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
@@ -840,7 +852,7 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
@@ -848,7 +860,7 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="2"/>
-        <v>8669850</v>
+        <v>345432</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
@@ -860,15 +872,15 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="3"/>
-        <v>3770000</v>
+        <v>2491000</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="1"/>
@@ -876,11 +888,11 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="2"/>
-        <v>4219938</v>
+        <v>3283665</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
@@ -892,11 +904,11 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="3"/>
-        <v>135000</v>
+        <v>9302000</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
@@ -904,15 +916,15 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="2"/>
-        <v>248343</v>
+        <v>12160690</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
@@ -924,7 +936,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="3"/>
-        <v>1480000</v>
+        <v>8755000</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
@@ -932,7 +944,7 @@
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
@@ -944,7 +956,7 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="2"/>
-        <v>1673199.0000000002</v>
+        <v>9725825</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -956,11 +968,11 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="3"/>
-        <v>1623000</v>
+        <v>5158000</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
@@ -968,15 +980,15 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="2"/>
-        <v>1853565.0000000002</v>
+        <v>5771318</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
@@ -988,11 +1000,11 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="3"/>
-        <v>3670000</v>
+        <v>2731000</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
@@ -1000,15 +1012,15 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="2"/>
-        <v>5150130</v>
+        <v>3298024</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
@@ -1020,7 +1032,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="3"/>
-        <v>317000</v>
+        <v>7303000</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
@@ -1036,11 +1048,11 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="2"/>
-        <v>503188</v>
+        <v>9566168</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
@@ -1052,15 +1064,15 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="3"/>
-        <v>4728000</v>
+        <v>1992000</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
@@ -1072,7 +1084,7 @@
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="2"/>
-        <v>6689763</v>
+        <v>2204198</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
@@ -1084,11 +1096,11 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="3"/>
-        <v>500000</v>
+        <v>7074000</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
@@ -1096,15 +1108,15 @@
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="2"/>
-        <v>573545</v>
+        <v>9294112</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
@@ -1116,15 +1128,15 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="3"/>
-        <v>5975000</v>
+        <v>9157000</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
@@ -1136,7 +1148,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="2"/>
-        <v>6649038.0000000009</v>
+        <v>9184595</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
@@ -1148,15 +1160,15 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="3"/>
-        <v>214000</v>
+        <v>5033000</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
@@ -1164,11 +1176,11 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="2"/>
-        <v>316450</v>
+        <v>5621570</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
@@ -1180,27 +1192,27 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="3"/>
-        <v>6181000</v>
+        <v>9653000</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="2"/>
-        <v>6246944</v>
+        <v>9665704</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -1212,7 +1224,7 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="3"/>
-        <v>8668000</v>
+        <v>5536000</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
@@ -1220,7 +1232,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
@@ -1232,7 +1244,7 @@
       </c>
       <c r="I26">
         <f t="shared" ca="1" si="2"/>
-        <v>11288808</v>
+        <v>7266394</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
@@ -1244,15 +1256,15 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="3"/>
-        <v>6496000</v>
+        <v>2246000</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
@@ -1260,11 +1272,11 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <f t="shared" ca="1" si="2"/>
-        <v>7201157.0000000009</v>
+        <v>2764599</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
@@ -1276,11 +1288,11 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="3"/>
-        <v>1983000</v>
+        <v>7243000</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
@@ -1288,7 +1300,7 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
@@ -1296,7 +1308,7 @@
       </c>
       <c r="I28">
         <f t="shared" ca="1" si="2"/>
-        <v>2231212</v>
+        <v>9443115</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -1308,7 +1320,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="3"/>
-        <v>6550000</v>
+        <v>4157000</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
@@ -1316,11 +1328,11 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
@@ -1328,7 +1340,7 @@
       </c>
       <c r="I29">
         <f t="shared" ca="1" si="2"/>
-        <v>9919336</v>
+        <v>4204021</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
@@ -1340,11 +1352,11 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="3"/>
-        <v>143000</v>
+        <v>556000</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
@@ -1356,11 +1368,11 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <f t="shared" ca="1" si="2"/>
-        <v>144460</v>
+        <v>644327</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
@@ -1372,11 +1384,11 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="3"/>
-        <v>8338000</v>
+        <v>7279000</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
@@ -1388,11 +1400,11 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <f t="shared" ca="1" si="2"/>
-        <v>11696272</v>
+        <v>9461013</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
@@ -1404,11 +1416,11 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="3"/>
-        <v>190000</v>
+        <v>7878000</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
@@ -1420,11 +1432,11 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <f t="shared" ca="1" si="2"/>
-        <v>305582</v>
+        <v>11055053</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
@@ -1436,19 +1448,19 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="3"/>
-        <v>6527000</v>
+        <v>3204000</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
@@ -1456,7 +1468,7 @@
       </c>
       <c r="I33">
         <f t="shared" ca="1" si="2"/>
-        <v>8506418</v>
+        <v>4257661</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
@@ -1468,27 +1480,27 @@
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="3"/>
-        <v>772000</v>
+        <v>8556000</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <f t="shared" ca="1" si="2"/>
-        <v>1008248</v>
+        <v>11136551</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
@@ -1500,11 +1512,11 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="3"/>
-        <v>8681000</v>
+        <v>7675000</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
@@ -1520,7 +1532,7 @@
       </c>
       <c r="I35">
         <f t="shared" ca="1" si="2"/>
-        <v>9647944</v>
+        <v>10064740</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
@@ -1532,11 +1544,11 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="3"/>
-        <v>1182000</v>
+        <v>4562000</v>
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="1"/>
@@ -1544,7 +1556,7 @@
       </c>
       <c r="G36">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
@@ -1552,7 +1564,7 @@
       </c>
       <c r="I36">
         <f t="shared" ref="I36:I67" ca="1" si="4">((RANDBETWEEN(10,15)/10)*D36)+(RANDBETWEEN(2000,4000)*E36)+(50000*F36)+(10000*G36)+(10000*H36)-(5000*C36)</f>
-        <v>1568820</v>
+        <v>6864240</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
@@ -1564,15 +1576,15 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="3"/>
-        <v>3022000</v>
+        <v>8599000</v>
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <f t="shared" ca="1" si="1"/>
@@ -1584,7 +1596,7 @@
       </c>
       <c r="I37">
         <f t="shared" ca="1" si="4"/>
-        <v>3947010</v>
+        <v>8661464</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
@@ -1596,11 +1608,11 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="3"/>
-        <v>6530000</v>
+        <v>8019000</v>
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="1"/>
@@ -1608,7 +1620,7 @@
       </c>
       <c r="G38">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
@@ -1616,7 +1628,7 @@
       </c>
       <c r="I38">
         <f t="shared" ca="1" si="4"/>
-        <v>7952595</v>
+        <v>8108080</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
@@ -1628,15 +1640,15 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="3"/>
-        <v>5006000</v>
+        <v>4957000</v>
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F39">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <f t="shared" ca="1" si="1"/>
@@ -1648,7 +1660,7 @@
       </c>
       <c r="I39">
         <f t="shared" ca="1" si="4"/>
-        <v>5058966</v>
+        <v>6027965</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
@@ -1660,11 +1672,11 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="3"/>
-        <v>631000</v>
+        <v>7741000</v>
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="1"/>
@@ -1680,7 +1692,7 @@
       </c>
       <c r="I40">
         <f t="shared" ca="1" si="4"/>
-        <v>925795</v>
+        <v>7762885</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
@@ -1692,19 +1704,19 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="3"/>
-        <v>9108000</v>
+        <v>2807000</v>
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
@@ -1712,7 +1724,7 @@
       </c>
       <c r="I41">
         <f t="shared" ca="1" si="4"/>
-        <v>12814520</v>
+        <v>3972929.9999999995</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
@@ -1724,15 +1736,15 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="3"/>
-        <v>1663000</v>
+        <v>8468000</v>
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <f t="shared" ca="1" si="1"/>
@@ -1740,11 +1752,11 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <f t="shared" ca="1" si="4"/>
-        <v>2399700</v>
+        <v>10207360</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
@@ -1756,11 +1768,11 @@
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="3"/>
-        <v>3713000</v>
+        <v>2585000</v>
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <f t="shared" ca="1" si="1"/>
@@ -1776,7 +1788,7 @@
       </c>
       <c r="I43">
         <f t="shared" ca="1" si="4"/>
-        <v>4855988</v>
+        <v>3664344</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
@@ -1788,15 +1800,15 @@
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="3"/>
-        <v>4247000</v>
+        <v>3700000</v>
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
         <f t="shared" ca="1" si="1"/>
@@ -1808,7 +1820,7 @@
       </c>
       <c r="I44">
         <f t="shared" ca="1" si="4"/>
-        <v>5151825</v>
+        <v>3776780</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
@@ -1820,11 +1832,11 @@
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="3"/>
-        <v>1110000</v>
+        <v>6891000</v>
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="1"/>
@@ -1832,7 +1844,7 @@
       </c>
       <c r="G45">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
@@ -1840,7 +1852,7 @@
       </c>
       <c r="I45">
         <f t="shared" ca="1" si="4"/>
-        <v>1213585</v>
+        <v>6954192</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
@@ -1852,11 +1864,11 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="3"/>
-        <v>7102000</v>
+        <v>5096000</v>
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="1"/>
@@ -1868,11 +1880,11 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <f t="shared" ca="1" si="4"/>
-        <v>7852620.0000000009</v>
+        <v>7138205</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
@@ -1884,7 +1896,7 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="3"/>
-        <v>5173000</v>
+        <v>4512000</v>
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="0"/>
@@ -1896,7 +1908,7 @@
       </c>
       <c r="G47">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
@@ -1904,7 +1916,7 @@
       </c>
       <c r="I47">
         <f t="shared" ca="1" si="4"/>
-        <v>6267780</v>
+        <v>4563398</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
@@ -1916,11 +1928,11 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="3"/>
-        <v>4277000</v>
+        <v>4466000</v>
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="1"/>
@@ -1932,11 +1944,11 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48">
         <f t="shared" ca="1" si="4"/>
-        <v>5569800</v>
+        <v>6702904</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
@@ -1948,15 +1960,15 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="3"/>
-        <v>8760000</v>
+        <v>3295000</v>
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <f t="shared" ca="1" si="1"/>
@@ -1968,7 +1980,7 @@
       </c>
       <c r="I49">
         <f t="shared" ca="1" si="4"/>
-        <v>10580305</v>
+        <v>3310332</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
@@ -1980,19 +1992,19 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="3"/>
-        <v>8689000</v>
+        <v>2795000</v>
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
@@ -2000,7 +2012,7 @@
       </c>
       <c r="I50">
         <f t="shared" ca="1" si="4"/>
-        <v>10497468</v>
+        <v>4205105</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
@@ -2012,11 +2024,11 @@
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="3"/>
-        <v>6970000</v>
+        <v>2478000</v>
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="1"/>
@@ -2032,7 +2044,7 @@
       </c>
       <c r="I51">
         <f t="shared" ca="1" si="4"/>
-        <v>7025749</v>
+        <v>2533765</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
@@ -2044,15 +2056,15 @@
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="3"/>
-        <v>7415000</v>
+        <v>2218000</v>
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
         <f t="shared" ca="1" si="1"/>
@@ -2064,7 +2076,7 @@
       </c>
       <c r="I52">
         <f t="shared" ca="1" si="4"/>
-        <v>11206684</v>
+        <v>3363018</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
@@ -2076,11 +2088,11 @@
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="3"/>
-        <v>7459000</v>
+        <v>1615000</v>
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="1"/>
@@ -2088,15 +2100,15 @@
       </c>
       <c r="G53">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
         <f t="shared" ca="1" si="4"/>
-        <v>9811010</v>
+        <v>1993756</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.2">
@@ -2108,15 +2120,15 @@
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="3"/>
-        <v>1520000</v>
+        <v>8155000</v>
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <f t="shared" ca="1" si="1"/>
@@ -2128,7 +2140,7 @@
       </c>
       <c r="I54">
         <f t="shared" ca="1" si="4"/>
-        <v>1846168</v>
+        <v>10691996</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
@@ -2140,15 +2152,15 @@
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="3"/>
-        <v>7469000</v>
+        <v>7512000</v>
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55">
         <f t="shared" ca="1" si="1"/>
@@ -2156,11 +2168,11 @@
       </c>
       <c r="H55">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
         <f t="shared" ca="1" si="4"/>
-        <v>11291764</v>
+        <v>9031780</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
@@ -2172,11 +2184,11 @@
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="3"/>
-        <v>9972000</v>
+        <v>6221000</v>
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="1"/>
@@ -2184,7 +2196,7 @@
       </c>
       <c r="G56">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
         <f t="shared" ca="1" si="1"/>
@@ -2192,7 +2204,7 @@
       </c>
       <c r="I56">
         <f t="shared" ca="1" si="4"/>
-        <v>13049005</v>
+        <v>8812156</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
@@ -2204,11 +2216,11 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="3"/>
-        <v>3091000</v>
+        <v>8958000</v>
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="1"/>
@@ -2216,7 +2228,7 @@
       </c>
       <c r="G57">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <f t="shared" ca="1" si="1"/>
@@ -2224,7 +2236,7 @@
       </c>
       <c r="I57">
         <f t="shared" ca="1" si="4"/>
-        <v>3469097.0000000005</v>
+        <v>12554154</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
@@ -2236,15 +2248,15 @@
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="3"/>
-        <v>3106000</v>
+        <v>493000</v>
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F58">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <f t="shared" ca="1" si="1"/>
@@ -2256,7 +2268,7 @@
       </c>
       <c r="I58">
         <f t="shared" ca="1" si="4"/>
-        <v>4085744</v>
+        <v>649090</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
@@ -2268,15 +2280,15 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="3"/>
-        <v>9209000</v>
+        <v>285000</v>
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F59">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
         <f t="shared" ca="1" si="1"/>
@@ -2288,7 +2300,7 @@
       </c>
       <c r="I59">
         <f t="shared" ca="1" si="4"/>
-        <v>12957970</v>
+        <v>347491</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
@@ -2300,11 +2312,11 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="3"/>
-        <v>829000</v>
+        <v>8996000</v>
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="1"/>
@@ -2312,15 +2324,15 @@
       </c>
       <c r="G60">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60">
         <f t="shared" ca="1" si="4"/>
-        <v>924695</v>
+        <v>9083922</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
@@ -2332,15 +2344,15 @@
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="3"/>
-        <v>3111000</v>
+        <v>8494000</v>
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F61">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61">
         <f t="shared" ca="1" si="1"/>
@@ -2348,11 +2360,11 @@
       </c>
       <c r="H61">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
         <f t="shared" ca="1" si="4"/>
-        <v>3447930.0000000005</v>
+        <v>11123588</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
@@ -2364,11 +2376,11 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="3"/>
-        <v>8511000</v>
+        <v>6192000</v>
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F62">
         <f t="shared" ca="1" si="1"/>
@@ -2376,7 +2388,7 @@
       </c>
       <c r="G62">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <f t="shared" ca="1" si="1"/>
@@ -2384,7 +2396,7 @@
       </c>
       <c r="I62">
         <f t="shared" ca="1" si="4"/>
-        <v>9405928</v>
+        <v>6217815</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
@@ -2396,27 +2408,27 @@
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="3"/>
-        <v>7679000</v>
+        <v>3539000</v>
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F63">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63">
         <f t="shared" ca="1" si="4"/>
-        <v>10003590</v>
+        <v>3636966</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
@@ -2428,11 +2440,11 @@
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="3"/>
-        <v>9011000</v>
+        <v>6196000</v>
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F64">
         <f t="shared" ca="1" si="1"/>
@@ -2444,11 +2456,11 @@
       </c>
       <c r="H64">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64">
         <f t="shared" ca="1" si="4"/>
-        <v>11795632</v>
+        <v>8740119</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
@@ -2460,27 +2472,27 @@
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="3"/>
-        <v>9760000</v>
+        <v>9407000</v>
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F65">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <f t="shared" ca="1" si="4"/>
-        <v>9782592</v>
+        <v>10409660</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
@@ -2492,15 +2504,15 @@
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="3"/>
-        <v>6528000</v>
+        <v>3696000</v>
       </c>
       <c r="E66">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F66">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <f t="shared" ca="1" si="1"/>
@@ -2508,11 +2520,11 @@
       </c>
       <c r="H66">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
         <f t="shared" ca="1" si="4"/>
-        <v>7259310.0000000009</v>
+        <v>4821552</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
@@ -2524,15 +2536,15 @@
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="3"/>
-        <v>9719000</v>
+        <v>1459000</v>
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F67">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67">
         <f t="shared" ca="1" si="1"/>
@@ -2540,11 +2552,11 @@
       </c>
       <c r="H67">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
         <f t="shared" ca="1" si="4"/>
-        <v>9753754</v>
+        <v>1543128</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
@@ -2556,11 +2568,11 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="3"/>
-        <v>9804000</v>
+        <v>1382000</v>
       </c>
       <c r="E68">
         <f t="shared" ref="E68:E102" ca="1" si="5">RANDBETWEEN(1,15)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F68">
         <f t="shared" ref="F68:H102" ca="1" si="6">RANDBETWEEN(0,1)</f>
@@ -2568,7 +2580,7 @@
       </c>
       <c r="G68">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <f t="shared" ca="1" si="6"/>
@@ -2576,7 +2588,7 @@
       </c>
       <c r="I68">
         <f t="shared" ref="I68:I99" ca="1" si="7">((RANDBETWEEN(10,15)/10)*D68)+(RANDBETWEEN(2000,4000)*E68)+(50000*F68)+(10000*G68)+(10000*H68)-(5000*C68)</f>
-        <v>12765295</v>
+        <v>2115203</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
@@ -2588,11 +2600,11 @@
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="3"/>
-        <v>2815000</v>
+        <v>6738000</v>
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F69">
         <f t="shared" ca="1" si="6"/>
@@ -2604,11 +2616,11 @@
       </c>
       <c r="H69">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69">
         <f t="shared" ca="1" si="7"/>
-        <v>3114452.0000000005</v>
+        <v>8083652</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
@@ -2620,11 +2632,11 @@
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="3"/>
-        <v>8675000</v>
+        <v>4247000</v>
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F70">
         <f t="shared" ca="1" si="6"/>
@@ -2640,7 +2652,7 @@
       </c>
       <c r="I70">
         <f t="shared" ca="1" si="7"/>
-        <v>9543788</v>
+        <v>5942989</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
@@ -2652,15 +2664,15 @@
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="3"/>
-        <v>6781000</v>
+        <v>4548000</v>
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F71">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <f t="shared" ca="1" si="6"/>
@@ -2672,7 +2684,7 @@
       </c>
       <c r="I71">
         <f t="shared" ca="1" si="7"/>
-        <v>9515152</v>
+        <v>6444976</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
@@ -2684,27 +2696,27 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="3"/>
-        <v>6220000</v>
+        <v>1619000</v>
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F72">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72">
         <f t="shared" ca="1" si="7"/>
-        <v>6931256.0000000009</v>
+        <v>1798141.0000000002</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
@@ -2716,15 +2728,15 @@
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="3"/>
-        <v>2052000</v>
+        <v>3018000</v>
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F73">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73">
         <f t="shared" ca="1" si="6"/>
@@ -2736,7 +2748,7 @@
       </c>
       <c r="I73">
         <f t="shared" ca="1" si="7"/>
-        <v>2490180</v>
+        <v>3140485</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
@@ -2748,7 +2760,7 @@
       </c>
       <c r="D74">
         <f t="shared" ref="D74:D102" ca="1" si="8">RANDBETWEEN(100,10000)*1000</f>
-        <v>4484000</v>
+        <v>2228000</v>
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="5"/>
@@ -2756,11 +2768,11 @@
       </c>
       <c r="F74">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <f t="shared" ca="1" si="6"/>
@@ -2768,7 +2780,7 @@
       </c>
       <c r="I74">
         <f t="shared" ca="1" si="7"/>
-        <v>5878565</v>
+        <v>3450630</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
@@ -2780,15 +2792,15 @@
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="8"/>
-        <v>5752000</v>
+        <v>8429000</v>
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F75">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75">
         <f t="shared" ca="1" si="6"/>
@@ -2796,11 +2808,11 @@
       </c>
       <c r="H75">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75">
         <f t="shared" ca="1" si="7"/>
-        <v>7549955</v>
+        <v>12666642</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
@@ -2812,27 +2824,27 @@
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="8"/>
-        <v>1403000</v>
+        <v>3590000</v>
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F76">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76">
         <f t="shared" ca="1" si="7"/>
-        <v>2160056</v>
+        <v>4733408</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
@@ -2844,15 +2856,15 @@
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="8"/>
-        <v>4175000</v>
+        <v>7465000</v>
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F77">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77">
         <f t="shared" ca="1" si="6"/>
@@ -2860,11 +2872,11 @@
       </c>
       <c r="H77">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77">
         <f t="shared" ca="1" si="7"/>
-        <v>4277628</v>
+        <v>8233170.0000000009</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
@@ -2876,11 +2888,11 @@
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="8"/>
-        <v>6889000</v>
+        <v>6478000</v>
       </c>
       <c r="E78">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F78">
         <f t="shared" ca="1" si="6"/>
@@ -2892,11 +2904,11 @@
       </c>
       <c r="H78">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78">
         <f t="shared" ca="1" si="7"/>
-        <v>8296264</v>
+        <v>9768480</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
@@ -2908,15 +2920,15 @@
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="8"/>
-        <v>4227000</v>
+        <v>1566000</v>
       </c>
       <c r="E79">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F79">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79">
         <f t="shared" ca="1" si="6"/>
@@ -2928,7 +2940,7 @@
       </c>
       <c r="I79">
         <f t="shared" ca="1" si="7"/>
-        <v>4702704</v>
+        <v>1782276.0000000002</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
@@ -2940,11 +2952,11 @@
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="8"/>
-        <v>7408000</v>
+        <v>5763000</v>
       </c>
       <c r="E80">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F80">
         <f t="shared" ca="1" si="6"/>
@@ -2952,15 +2964,15 @@
       </c>
       <c r="G80">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80">
         <f t="shared" ca="1" si="7"/>
-        <v>8943930</v>
+        <v>8094547.9999999991</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
@@ -2972,11 +2984,11 @@
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="8"/>
-        <v>1925000</v>
+        <v>3715000</v>
       </c>
       <c r="E81">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F81">
         <f t="shared" ca="1" si="6"/>
@@ -2984,15 +2996,15 @@
       </c>
       <c r="G81">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81">
         <f t="shared" ca="1" si="7"/>
-        <v>2528898</v>
+        <v>5240369</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
@@ -3004,7 +3016,7 @@
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="8"/>
-        <v>4383000</v>
+        <v>1081000</v>
       </c>
       <c r="E82">
         <f t="shared" ca="1" si="5"/>
@@ -3024,7 +3036,7 @@
       </c>
       <c r="I82">
         <f t="shared" ca="1" si="7"/>
-        <v>4878242</v>
+        <v>1577258</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
@@ -3036,11 +3048,11 @@
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="8"/>
-        <v>9289000</v>
+        <v>686000</v>
       </c>
       <c r="E83">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F83">
         <f t="shared" ca="1" si="6"/>
@@ -3056,7 +3068,7 @@
       </c>
       <c r="I83">
         <f t="shared" ca="1" si="7"/>
-        <v>9350715</v>
+        <v>770620.00000000012</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
@@ -3068,11 +3080,11 @@
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="8"/>
-        <v>6607000</v>
+        <v>3843000</v>
       </c>
       <c r="E84">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F84">
         <f t="shared" ca="1" si="6"/>
@@ -3088,7 +3100,7 @@
       </c>
       <c r="I84">
         <f t="shared" ca="1" si="7"/>
-        <v>9918967</v>
+        <v>4662248</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
@@ -3100,11 +3112,11 @@
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="8"/>
-        <v>8143000</v>
+        <v>1389000</v>
       </c>
       <c r="E85">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F85">
         <f t="shared" ca="1" si="6"/>
@@ -3112,7 +3124,7 @@
       </c>
       <c r="G85">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85">
         <f t="shared" ca="1" si="6"/>
@@ -3120,7 +3132,7 @@
       </c>
       <c r="I85">
         <f t="shared" ca="1" si="7"/>
-        <v>8212922</v>
+        <v>2186716</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
@@ -3132,7 +3144,7 @@
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="8"/>
-        <v>7409000</v>
+        <v>7975000</v>
       </c>
       <c r="E86">
         <f t="shared" ca="1" si="5"/>
@@ -3140,11 +3152,11 @@
       </c>
       <c r="F86">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <f t="shared" ca="1" si="6"/>
@@ -3152,7 +3164,7 @@
       </c>
       <c r="I86">
         <f t="shared" ca="1" si="7"/>
-        <v>7510800</v>
+        <v>9615947</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
@@ -3164,27 +3176,27 @@
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="8"/>
-        <v>6986000</v>
+        <v>1597000</v>
       </c>
       <c r="E87">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F87">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I87">
         <f t="shared" ca="1" si="7"/>
-        <v>7011310</v>
+        <v>1973884</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
@@ -3196,11 +3208,11 @@
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="8"/>
-        <v>930000</v>
+        <v>765000</v>
       </c>
       <c r="E88">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F88">
         <f t="shared" ca="1" si="6"/>
@@ -3208,7 +3220,7 @@
       </c>
       <c r="G88">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <f t="shared" ca="1" si="6"/>
@@ -3216,7 +3228,7 @@
       </c>
       <c r="I88">
         <f t="shared" ca="1" si="7"/>
-        <v>1222848</v>
+        <v>1023208</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
@@ -3228,19 +3240,19 @@
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="8"/>
-        <v>8283000</v>
+        <v>1115000</v>
       </c>
       <c r="E89">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F89">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <f t="shared" ca="1" si="6"/>
@@ -3248,7 +3260,7 @@
       </c>
       <c r="I89">
         <f t="shared" ca="1" si="7"/>
-        <v>11685958</v>
+        <v>1154772</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
@@ -3260,27 +3272,27 @@
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="8"/>
-        <v>1041000</v>
+        <v>6684000</v>
       </c>
       <c r="E90">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F90">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I90">
         <f t="shared" ca="1" si="7"/>
-        <v>1362784</v>
+        <v>9445160</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
@@ -3292,15 +3304,15 @@
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="8"/>
-        <v>8117000</v>
+        <v>950000</v>
       </c>
       <c r="E91">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F91">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91">
         <f t="shared" ca="1" si="6"/>
@@ -3312,7 +3324,7 @@
       </c>
       <c r="I91">
         <f t="shared" ca="1" si="7"/>
-        <v>10649676</v>
+        <v>962785</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
@@ -3324,11 +3336,11 @@
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="8"/>
-        <v>5722000</v>
+        <v>635000</v>
       </c>
       <c r="E92">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F92">
         <f t="shared" ca="1" si="6"/>
@@ -3336,7 +3348,7 @@
       </c>
       <c r="G92">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92">
         <f t="shared" ca="1" si="6"/>
@@ -3344,7 +3356,7 @@
       </c>
       <c r="I92">
         <f t="shared" ca="1" si="7"/>
-        <v>7463365</v>
+        <v>999056</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
@@ -3356,11 +3368,11 @@
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="8"/>
-        <v>8096000</v>
+        <v>8346000</v>
       </c>
       <c r="E93">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F93">
         <f t="shared" ca="1" si="6"/>
@@ -3376,7 +3388,7 @@
       </c>
       <c r="I93">
         <f t="shared" ca="1" si="7"/>
-        <v>10570152</v>
+        <v>10042915</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
@@ -3388,11 +3400,11 @@
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="8"/>
-        <v>9248000</v>
+        <v>3054000</v>
       </c>
       <c r="E94">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F94">
         <f t="shared" ca="1" si="6"/>
@@ -3400,7 +3412,7 @@
       </c>
       <c r="G94">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
         <f t="shared" ca="1" si="6"/>
@@ -3408,7 +3420,7 @@
       </c>
       <c r="I94">
         <f t="shared" ca="1" si="7"/>
-        <v>11158525</v>
+        <v>3683365</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
@@ -3420,11 +3432,11 @@
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="8"/>
-        <v>7669000</v>
+        <v>4870000</v>
       </c>
       <c r="E95">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F95">
         <f t="shared" ca="1" si="6"/>
@@ -3432,15 +3444,15 @@
       </c>
       <c r="G95">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95">
         <f t="shared" ca="1" si="7"/>
-        <v>7693332</v>
+        <v>5393900</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
@@ -3452,19 +3464,19 @@
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="8"/>
-        <v>610000</v>
+        <v>1122000</v>
       </c>
       <c r="E96">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F96">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96">
         <f t="shared" ca="1" si="6"/>
@@ -3472,7 +3484,7 @@
       </c>
       <c r="I96">
         <f t="shared" ca="1" si="7"/>
-        <v>615414</v>
+        <v>1424844</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.2">
@@ -3484,11 +3496,11 @@
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="8"/>
-        <v>1203000</v>
+        <v>7967000</v>
       </c>
       <c r="E97">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F97">
         <f t="shared" ca="1" si="6"/>
@@ -3500,11 +3512,11 @@
       </c>
       <c r="H97">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97">
         <f t="shared" ca="1" si="7"/>
-        <v>1636800</v>
+        <v>12041900</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.2">
@@ -3516,27 +3528,27 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="8"/>
-        <v>1079000</v>
+        <v>711000</v>
       </c>
       <c r="E98">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F98">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98">
         <f t="shared" ca="1" si="7"/>
-        <v>1704710</v>
+        <v>909720</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.2">
@@ -3548,11 +3560,11 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="8"/>
-        <v>647000</v>
+        <v>6440000</v>
       </c>
       <c r="E99">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F99">
         <f t="shared" ca="1" si="6"/>
@@ -3568,7 +3580,7 @@
       </c>
       <c r="I99">
         <f t="shared" ca="1" si="7"/>
-        <v>1007210</v>
+        <v>8475572</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.2">
@@ -3580,15 +3592,15 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="8"/>
-        <v>6472000</v>
+        <v>1215000</v>
       </c>
       <c r="E100">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F100">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100">
         <f t="shared" ca="1" si="6"/>
@@ -3600,7 +3612,7 @@
       </c>
       <c r="I100">
         <f t="shared" ref="I100:I102" ca="1" si="9">((RANDBETWEEN(10,15)/10)*D100)+(RANDBETWEEN(2000,4000)*E100)+(50000*F100)+(10000*G100)+(10000*H100)-(5000*C100)</f>
-        <v>8476926</v>
+        <v>1725305</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.2">
@@ -3612,11 +3624,11 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="8"/>
-        <v>4625000</v>
+        <v>3219000</v>
       </c>
       <c r="E101">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F101">
         <f t="shared" ca="1" si="6"/>
@@ -3628,11 +3640,11 @@
       </c>
       <c r="H101">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101">
         <f t="shared" ca="1" si="9"/>
-        <v>6105470</v>
+        <v>3935216</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.2">
@@ -3644,11 +3656,11 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="8"/>
-        <v>2707000</v>
+        <v>9362000</v>
       </c>
       <c r="E102">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F102">
         <f t="shared" ca="1" si="6"/>
@@ -3664,7 +3676,7 @@
       </c>
       <c r="I102">
         <f t="shared" ca="1" si="9"/>
-        <v>2774730</v>
+        <v>12227548</v>
       </c>
     </row>
   </sheetData>
@@ -3677,7 +3689,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H101"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3696,22 +3708,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -3741,7 +3753,7 @@
       </c>
       <c r="H2" s="2">
         <f ca="1">((RANDBETWEEN(10,16)/100)*C2)+(IF(D2 &lt; 5, D2 * RANDBETWEEN(75, 90)/100, D2 * RANDBETWEEN(100, 115)/100))+(20000*E2)+(10000*F2)+(10000*G2)-(5000*B2)</f>
-        <v>70005.2</v>
+        <v>65005.25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3768,7 +3780,7 @@
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H66" ca="1" si="0">((RANDBETWEEN(10,16)/100)*C3)+(IF(D3 &lt; 5, D3 * RANDBETWEEN(75, 90)/100, D3 * RANDBETWEEN(100, 115)/100))+(20000*E3)+(10000*F3)+(10000*G3)-(5000*B3)</f>
-        <v>15001.8</v>
+        <v>19001.580000000002</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3795,7 +3807,7 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>105007.7</v>
+        <v>135007.91</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -3822,7 +3834,7 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>93006.9</v>
+        <v>99006.720000000016</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3849,7 +3861,7 @@
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>49013.26</v>
+        <v>58014.040000000008</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3876,7 +3888,7 @@
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1325002.25</v>
+        <v>1525002.55</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3903,7 +3915,7 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>216183.00000000003</v>
+        <v>216183.36000000002</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -3930,7 +3942,7 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>751181.22</v>
+        <v>806272.43000000017</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -3957,7 +3969,7 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>921303.12</v>
+        <v>1187193.48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3984,7 +3996,7 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1219508.56</v>
+        <v>1219509.04</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4011,7 +4023,7 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>136301.68</v>
+        <v>199451.76</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -4038,7 +4050,7 @@
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>845841.68</v>
+        <v>914661.62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -4065,7 +4077,7 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>383200.78</v>
+        <v>292400.82</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -4092,7 +4104,7 @@
       </c>
       <c r="H15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>772935</v>
+        <v>972825.55000000016</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -4119,7 +4131,7 @@
       </c>
       <c r="H16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>131411.99</v>
+        <v>167832.65</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -4146,7 +4158,7 @@
       </c>
       <c r="H17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>883393.91</v>
+        <v>1271294.43</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -4173,7 +4185,7 @@
       </c>
       <c r="H18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>956416.05</v>
+        <v>709375</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -4200,7 +4212,7 @@
       </c>
       <c r="H19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>414970.2</v>
+        <v>518710.4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4227,7 +4239,7 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1350654.69</v>
+        <v>937954.17</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -4254,7 +4266,7 @@
       </c>
       <c r="H21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>503247.35</v>
+        <v>583787.84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -4281,7 +4293,7 @@
       </c>
       <c r="H22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>720415.54</v>
+        <v>776214.70000000007</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -4308,7 +4320,7 @@
       </c>
       <c r="H23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>406306.42</v>
+        <v>529696.78</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -4335,7 +4347,7 @@
       </c>
       <c r="H24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1152901.58</v>
+        <v>1329501.58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -4362,7 +4374,7 @@
       </c>
       <c r="H25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1201414.69</v>
+        <v>1201414.3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -4389,7 +4401,7 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1284982.24</v>
+        <v>991913.2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -4416,7 +4428,7 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>55547.490000000005</v>
+        <v>55547.070000000007</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -4443,7 +4455,7 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>555560.9</v>
+        <v>684920.75</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -4470,7 +4482,7 @@
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>800853</v>
+        <v>651634.94999999995</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4497,7 +4509,7 @@
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>22423</v>
+        <v>22423.119999999999</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -4524,7 +4536,7 @@
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>893933.13</v>
+        <v>966344.17</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -4551,7 +4563,7 @@
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>741955.7</v>
+        <v>741955.45</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -4578,7 +4590,7 @@
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>120706.78</v>
+        <v>105946.24000000001</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -4605,7 +4617,7 @@
       </c>
       <c r="H34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>496758.56</v>
+        <v>496758.96</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4632,7 +4644,7 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>531870.5</v>
+        <v>379910.8</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -4659,7 +4671,7 @@
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1436487.56</v>
+        <v>1436487.14</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -4686,7 +4698,7 @@
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1132566.72</v>
+        <v>1219686.18</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -4713,7 +4725,7 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1076561</v>
+        <v>1076560.2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -4740,7 +4752,7 @@
       </c>
       <c r="H39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>260001.58</v>
+        <v>243751.66</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -4767,7 +4779,7 @@
       </c>
       <c r="H40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>168256.35</v>
+        <v>168257.25</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -4794,7 +4806,7 @@
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>785371.88</v>
+        <v>688452.10000000009</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -4821,7 +4833,7 @@
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>194443.56</v>
+        <v>230703.8</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -4848,7 +4860,7 @@
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>890701.76000000013</v>
+        <v>828151.6</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -4875,7 +4887,7 @@
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>816590.10000000009</v>
+        <v>584710.6</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -4902,7 +4914,7 @@
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>204690.35</v>
+        <v>204689.27</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -4929,7 +4941,7 @@
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1077812.3600000001</v>
+        <v>1077813.08</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -4956,7 +4968,7 @@
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>908687.00000000012</v>
+        <v>782447.63</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -4983,7 +4995,7 @@
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1127840.8400000001</v>
+        <v>1502120.8</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -5010,7 +5022,7 @@
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1020820.81</v>
+        <v>786400.78</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -5037,7 +5049,7 @@
       </c>
       <c r="H50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>308808.05</v>
+        <v>308807.42</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -5064,7 +5076,7 @@
       </c>
       <c r="H51" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>382674.98000000004</v>
+        <v>382675.54000000004</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -5091,7 +5103,7 @@
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1003220.9000000001</v>
+        <v>792530.76</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -5118,7 +5130,7 @@
       </c>
       <c r="H53" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1036888.08</v>
+        <v>1291108.6399999999</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -5145,7 +5157,7 @@
       </c>
       <c r="H54" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1128122.55</v>
+        <v>1128122.43</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -5172,7 +5184,7 @@
       </c>
       <c r="H55" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>321960.7</v>
+        <v>321960.40000000002</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -5199,7 +5211,7 @@
       </c>
       <c r="H56" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>244616.65</v>
+        <v>334456.80000000005</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -5226,7 +5238,7 @@
       </c>
       <c r="H57" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>917600.86</v>
+        <v>917600.89</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -5253,7 +5265,7 @@
       </c>
       <c r="H58" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>65800.84</v>
+        <v>65800.78</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -5280,7 +5292,7 @@
       </c>
       <c r="H59" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>191880.9</v>
+        <v>177890.8</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -5307,7 +5319,7 @@
       </c>
       <c r="H60" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>207465.3</v>
+        <v>301765.40000000002</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -5334,7 +5346,7 @@
       </c>
       <c r="H61" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>972299.9</v>
+        <v>1237470.0800000003</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -5361,7 +5373,7 @@
       </c>
       <c r="H62" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>532402.43000000005</v>
+        <v>576352.31000000006</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -5388,7 +5400,7 @@
       </c>
       <c r="H63" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>601528.16</v>
+        <v>800369.04</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -5415,7 +5427,7 @@
       </c>
       <c r="H64" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>426931.1</v>
+        <v>295081.40000000002</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -5442,7 +5454,7 @@
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>142165.29999999999</v>
+        <v>187885.05</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -5469,7 +5481,7 @@
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>39096.78</v>
+        <v>36906.9</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -5496,7 +5508,7 @@
       </c>
       <c r="H67" s="2">
         <f t="shared" ref="H67:H101" ca="1" si="1">((RANDBETWEEN(10,16)/100)*C67)+(IF(D67 &lt; 5, D67 * RANDBETWEEN(75, 90)/100, D67 * RANDBETWEEN(100, 115)/100))+(20000*E67)+(10000*F67)+(10000*G67)-(5000*B67)</f>
-        <v>88612.43</v>
+        <v>130411.98999999999</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -5523,7 +5535,7 @@
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>752402.49</v>
+        <v>1043362.6700000002</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -5550,7 +5562,7 @@
       </c>
       <c r="H69" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1082316.8399999999</v>
+        <v>1082316.6600000001</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -5577,7 +5589,7 @@
       </c>
       <c r="H70" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>614613.56000000006</v>
+        <v>462212.72</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -5604,7 +5616,7 @@
       </c>
       <c r="H71" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>918513.68</v>
+        <v>1472612.36</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -5631,7 +5643,7 @@
       </c>
       <c r="H72" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>501531.4</v>
+        <v>665370.6</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -5658,7 +5670,7 @@
       </c>
       <c r="H73" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>793493.08</v>
+        <v>989362.12</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -5685,7 +5697,7 @@
       </c>
       <c r="H74" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1011265.54</v>
+        <v>858764.84</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -5712,7 +5724,7 @@
       </c>
       <c r="H75" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>443605.35</v>
+        <v>530325</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -5739,7 +5751,7 @@
       </c>
       <c r="H76" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1051847.7</v>
+        <v>883207.56</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -5766,7 +5778,7 @@
       </c>
       <c r="H77" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>442400.8</v>
+        <v>374340.5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -5793,7 +5805,7 @@
       </c>
       <c r="H78" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>835849</v>
+        <v>733870.35000000009</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -5820,7 +5832,7 @@
       </c>
       <c r="H79" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>590328.4</v>
+        <v>372708.96</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -5847,7 +5859,7 @@
       </c>
       <c r="H80" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>374403.2</v>
+        <v>468003.24</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -5874,7 +5886,7 @@
       </c>
       <c r="H81" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>221329.54000000004</v>
+        <v>235709.45</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -5901,7 +5913,7 @@
       </c>
       <c r="H82" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1513417.1</v>
+        <v>1138815.45</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -5928,7 +5940,7 @@
       </c>
       <c r="H83" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>336211.77</v>
+        <v>274112.65000000002</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -5955,7 +5967,7 @@
       </c>
       <c r="H84" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>585252.25</v>
+        <v>796252.34</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -5982,7 +5994,7 @@
       </c>
       <c r="H85" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>353373.52</v>
+        <v>295313</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -6009,7 +6021,7 @@
       </c>
       <c r="H86" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>248561.44</v>
+        <v>201851</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -6036,7 +6048,7 @@
       </c>
       <c r="H87" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1036932.46</v>
+        <v>958322.37</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -6063,7 +6075,7 @@
       </c>
       <c r="H88" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>37214.43</v>
+        <v>40434.04</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -6090,7 +6102,7 @@
       </c>
       <c r="H89" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>528895.6</v>
+        <v>573386.35</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -6117,7 +6129,7 @@
       </c>
       <c r="H90" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>454130.82</v>
+        <v>535790.89</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -6144,7 +6156,7 @@
       </c>
       <c r="H91" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1095712.32</v>
+        <v>927911.88</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -6171,7 +6183,7 @@
       </c>
       <c r="H92" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>237853.48</v>
+        <v>207473.24</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -6198,7 +6210,7 @@
       </c>
       <c r="H93" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>516331.74</v>
+        <v>470301.68</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -6225,7 +6237,7 @@
       </c>
       <c r="H94" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1053907.42</v>
+        <v>1053907.28</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -6252,7 +6264,7 @@
       </c>
       <c r="H95" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>526302.37</v>
+        <v>491882.55000000005</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -6279,7 +6291,7 @@
       </c>
       <c r="H96" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>920712.96</v>
+        <v>861333.56000000017</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -6306,7 +6318,7 @@
       </c>
       <c r="H97" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>312814.3</v>
+        <v>215064.95</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -6333,7 +6345,7 @@
       </c>
       <c r="H98" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>851153.32</v>
+        <v>1224403.24</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -6360,7 +6372,7 @@
       </c>
       <c r="H99" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>523902.61</v>
+        <v>780852.4</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -6387,7 +6399,7 @@
       </c>
       <c r="H100" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>201609.81000000003</v>
+        <v>201609.27000000002</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -6414,7 +6426,7 @@
       </c>
       <c r="H101" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1410557.77</v>
+        <v>1410557.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>